<commit_message>
Update cosc 3506 001x group members.xlsx
updated to full 4 member version
</commit_message>
<xml_diff>
--- a/cosc 3506 001x group members.xlsx
+++ b/cosc 3506 001x group members.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/27a95698cb5d55a1/桌面/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/27a95698cb5d55a1/文档/GitHub/groupproj_3506/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F83D3167-5F45-4D03-A9E4-B0ADAA9CFFA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6F84B3F9-18BE-4E3D-8A12-396930E1F995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="1" xr2:uid="{95510D40-55B8-44B2-9E3E-D3470FC5973B}"/>
   </bookViews>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
   <si>
     <t>Member</t>
   </si>
@@ -84,9 +84,6 @@
   </si>
   <si>
     <t>Course (COSC/ITEC)</t>
-  </si>
-  <si>
-    <t>All must be from same course</t>
   </si>
   <si>
     <t>Section</t>
@@ -135,12 +132,24 @@
     <t>tjohnson@algomau.ca</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>Cordelle WaldenCameron</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cwaldencameron@algomau.ca</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>All must be from same course</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -170,14 +179,6 @@
       <color rgb="FF000000"/>
       <name val="等线"/>
       <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -222,7 +223,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -307,49 +308,68 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="medium">
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -360,7 +380,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -394,13 +414,14 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1004,10 +1025,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12CFCCA7-E07C-4D05-8125-DC07B6CB2043}">
-  <dimension ref="F2:K9"/>
+  <dimension ref="F3:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="F3" sqref="F3:K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1019,111 +1040,117 @@
     <col min="11" max="11" width="26.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="6:11" ht="14.5" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="6:11" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="6:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F3" s="14" t="s">
         <v>0</v>
       </c>
       <c r="G3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="H3" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="I3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="14" t="s">
+      <c r="J3" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="K3" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="14" t="s">
+    </row>
+    <row r="4" spans="6:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="16"/>
+      <c r="K4" s="14"/>
+    </row>
+    <row r="5" spans="6:11" x14ac:dyDescent="0.3">
+      <c r="F5" s="11">
+        <v>1</v>
+      </c>
+      <c r="G5" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="6:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="13" t="s">
+      <c r="H5" s="11">
+        <v>249561910</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="6:11" x14ac:dyDescent="0.3">
+      <c r="F6" s="11">
+        <v>2</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="11">
+        <v>249529030</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="6:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F7" s="11">
+        <v>3</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="11">
+        <v>219632800</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="J7" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K7" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="6:11" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F8" s="11">
         <v>4</v>
       </c>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
-    </row>
-    <row r="5" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5" t="s">
-        <v>7</v>
-      </c>
-      <c r="H5">
-        <v>249561910</v>
-      </c>
-      <c r="I5" t="s">
+      <c r="G8" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="11">
+        <v>249447300</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="J8" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="J5" t="s">
-        <v>11</v>
-      </c>
-      <c r="K5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F6">
-        <v>2</v>
-      </c>
-      <c r="G6" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6">
-        <v>249529030</v>
-      </c>
-      <c r="I6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="6:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F7">
-        <v>3</v>
-      </c>
-      <c r="G7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H7">
-        <v>219632800</v>
-      </c>
-      <c r="I7" t="s">
-        <v>10</v>
-      </c>
-      <c r="J7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="6:11" ht="14" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F8">
-        <v>4</v>
-      </c>
-      <c r="I8" t="s">
-        <v>10</v>
-      </c>
-      <c r="J8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="G9" s="11"/>
-    </row>
+      <c r="K8" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="6:11" ht="14" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="F3:F4"/>

</xml_diff>